<commit_message>
writing up and uploading SQL files
</commit_message>
<xml_diff>
--- a/Part 1/city sample check.xlsx
+++ b/Part 1/city sample check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theorogers/Desktop/SkillsyBits/Projects/SQL/CitiesXAltitude/Part 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8968B2-8CEB-5341-8435-2EF5E51BA8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6A7A5F-7BFD-D740-9F3A-D97B57FF2769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="2040" windowWidth="28040" windowHeight="16320" xr2:uid="{2F65151E-F47C-2641-932A-C3249709BA6D}"/>
+    <workbookView xWindow="980" yWindow="1120" windowWidth="28040" windowHeight="16340" xr2:uid="{2F65151E-F47C-2641-932A-C3249709BA6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -276,7 +276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -317,6 +317,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF001D35"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -347,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -380,11 +393,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -416,94 +431,12 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -523,44 +456,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1534,7 +1429,7 @@
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
                 <a:ln w="9525">
                   <a:noFill/>
@@ -4461,13 +4356,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34C2BCEB-D397-FA41-91A3-FFA45EA04A9A}" name="Table1" displayName="Table1" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34C2BCEB-D397-FA41-91A3-FFA45EA04A9A}" name="Table1" displayName="Table1" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:H1048576" xr:uid="{34C2BCEB-D397-FA41-91A3-FFA45EA04A9A}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7050CA82-6C89-A34C-BB77-A6B47F98D8E5}" name="Town"/>
     <tableColumn id="2" xr3:uid="{88748B05-AB7C-2B42-B19D-8AC3A8BAA83F}" name="Country"/>
-    <tableColumn id="3" xr3:uid="{97D7BF6C-8FC8-4448-935B-0D3BAE1C56AB}" name="PopSM" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{5C87B263-61E9-2A4B-B549-B12DEDEFC17F}" name="PopGN" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{97D7BF6C-8FC8-4448-935B-0D3BAE1C56AB}" name="PopSM" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{5C87B263-61E9-2A4B-B549-B12DEDEFC17F}" name="PopGN" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{9D7AB58D-FA3B-2F47-8F0C-265ECAB0E74B}" name="ALPR"/>
     <tableColumn id="6" xr3:uid="{174D6A3E-C80A-B24C-94E6-4EDCFB68E08E}" name="Haversine"/>
     <tableColumn id="7" xr3:uid="{94BA9740-8D09-FA4F-940E-8CC7C80FAC8D}" name="Log Haversine"/>
@@ -4796,8 +4691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D11A49-FB6A-2145-9B8B-AD1FA4C0CDCD}">
   <dimension ref="A1:S259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4884,7 +4779,7 @@
         <v>1.31</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G2:G65" si="0">LOG(F3+0.1)</f>
+        <f t="shared" ref="G3:G65" si="0">LOG(F3+0.1)</f>
         <v>0.14921911265537993</v>
       </c>
       <c r="H3" t="s">
@@ -4971,10 +4866,6 @@
       <c r="H6" t="s">
         <v>70</v>
       </c>
-      <c r="S6">
-        <f>LOG(10)</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -5083,10 +4974,6 @@
       <c r="H10" t="s">
         <v>70</v>
       </c>
-      <c r="S10">
-        <f>LOG(30)</f>
-        <v>1.4771212547196624</v>
-      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -5222,6 +5109,10 @@
       <c r="H15" t="s">
         <v>70</v>
       </c>
+      <c r="R15">
+        <f>31344-194</f>
+        <v>31150</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -5243,14 +5134,21 @@
         <v>0.15</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="0"/>
+        <f>LOG(F16+0.1)</f>
         <v>-0.6020599913279624</v>
       </c>
       <c r="H16" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R16">
+        <v>47802</v>
+      </c>
+      <c r="S16">
+        <f>(R16-R15)/R16</f>
+        <v>0.34835362537132336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -5277,7 +5175,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -5304,7 +5202,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -5331,7 +5229,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -5358,7 +5256,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -5385,7 +5283,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
@@ -5412,7 +5310,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
@@ -5438,8 +5336,9 @@
       <c r="H23" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -5466,7 +5365,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -5493,7 +5392,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -5520,7 +5419,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
@@ -5547,7 +5446,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -5574,7 +5473,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>51</v>
       </c>
@@ -5601,7 +5500,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
@@ -5628,7 +5527,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
@@ -5655,7 +5554,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>56</v>
       </c>
@@ -8908,7 +8807,7 @@
       </c>
       <c r="H160" s="11"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" s="13" t="s">
         <v>53</v>
       </c>
@@ -8933,7 +8832,7 @@
       </c>
       <c r="H161" s="11"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" s="13" t="s">
         <v>53</v>
       </c>
@@ -8958,7 +8857,7 @@
       </c>
       <c r="H162" s="11"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" ht="23" x14ac:dyDescent="0.25">
       <c r="A163" s="13" t="s">
         <v>53</v>
       </c>
@@ -8982,8 +8881,9 @@
         <v>3.2007492967804514</v>
       </c>
       <c r="H163" s="11"/>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K163" s="20"/>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" s="13" t="s">
         <v>53</v>
       </c>
@@ -9008,7 +8908,7 @@
       </c>
       <c r="H164" s="11"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" s="13" t="s">
         <v>53</v>
       </c>
@@ -9033,7 +8933,7 @@
       </c>
       <c r="H165" s="11"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" s="13" t="s">
         <v>53</v>
       </c>
@@ -9058,7 +8958,7 @@
       </c>
       <c r="H166" s="11"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" s="13" t="s">
         <v>53</v>
       </c>
@@ -9083,7 +8983,7 @@
       </c>
       <c r="H167" s="11"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" s="13" t="s">
         <v>53</v>
       </c>
@@ -9108,7 +9008,7 @@
       </c>
       <c r="H168" s="11"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" s="13" t="s">
         <v>53</v>
       </c>
@@ -9135,7 +9035,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" s="13" t="s">
         <v>53</v>
       </c>
@@ -9160,7 +9060,7 @@
       </c>
       <c r="H170" s="11"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" s="13" t="s">
         <v>53</v>
       </c>
@@ -9185,7 +9085,7 @@
       </c>
       <c r="H171" s="11"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" s="13" t="s">
         <v>53</v>
       </c>
@@ -9210,7 +9110,7 @@
       </c>
       <c r="H172" s="11"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" s="13" t="s">
         <v>53</v>
       </c>
@@ -9235,7 +9135,7 @@
       </c>
       <c r="H173" s="11"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" s="13" t="s">
         <v>53</v>
       </c>
@@ -9260,7 +9160,7 @@
       </c>
       <c r="H174" s="11"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" s="13" t="s">
         <v>53</v>
       </c>
@@ -9285,7 +9185,7 @@
       </c>
       <c r="H175" s="11"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" s="13" t="s">
         <v>53</v>
       </c>
@@ -9310,7 +9210,7 @@
       </c>
       <c r="H176" s="11"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" s="13" t="s">
         <v>53</v>
       </c>
@@ -9335,7 +9235,7 @@
       </c>
       <c r="H177" s="11"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" s="13" t="s">
         <v>53</v>
       </c>
@@ -9360,7 +9260,7 @@
       </c>
       <c r="H178" s="11"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" s="13" t="s">
         <v>53</v>
       </c>
@@ -9385,7 +9285,7 @@
       </c>
       <c r="H179" s="11"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" s="13" t="s">
         <v>53</v>
       </c>
@@ -9410,7 +9310,7 @@
       </c>
       <c r="H180" s="11"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" s="13" t="s">
         <v>53</v>
       </c>
@@ -9435,7 +9335,7 @@
       </c>
       <c r="H181" s="11"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" s="13" t="s">
         <v>53</v>
       </c>
@@ -9460,7 +9360,7 @@
       </c>
       <c r="H182" s="11"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" s="13" t="s">
         <v>53</v>
       </c>
@@ -9485,7 +9385,7 @@
       </c>
       <c r="H183" s="11"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" s="13" t="s">
         <v>53</v>
       </c>
@@ -9510,7 +9410,7 @@
       </c>
       <c r="H184" s="11"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" s="13" t="s">
         <v>53</v>
       </c>
@@ -9535,7 +9435,7 @@
       </c>
       <c r="H185" s="11"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" s="13" t="s">
         <v>53</v>
       </c>
@@ -9560,7 +9460,7 @@
       </c>
       <c r="H186" s="11"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" s="13" t="s">
         <v>53</v>
       </c>
@@ -9585,7 +9485,7 @@
       </c>
       <c r="H187" s="11"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" s="13" t="s">
         <v>53</v>
       </c>
@@ -9610,7 +9510,7 @@
       </c>
       <c r="H188" s="11"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" s="13" t="s">
         <v>53</v>
       </c>
@@ -9633,11 +9533,17 @@
         <f t="shared" si="2"/>
         <v>1.3289908554494287</v>
       </c>
-      <c r="H189" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H189" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="J189" s="1">
+        <v>1840152388</v>
+      </c>
+      <c r="K189" s="1">
+        <v>4561407</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" s="13" t="s">
         <v>53</v>
       </c>
@@ -9662,7 +9568,7 @@
       </c>
       <c r="H190" s="11"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" s="13" t="s">
         <v>53</v>
       </c>
@@ -9687,7 +9593,7 @@
       </c>
       <c r="H191" s="11"/>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" s="13" t="s">
         <v>53</v>
       </c>

</xml_diff>